<commit_message>
[GPR] Atualizações mínimas gerais.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Plano de Envolvimento.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Plano de Envolvimento.xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="25908"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciuscmac/Desktop/GitHub/P.I.-ES-UFG-2015-BIJLMMV/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="19780" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Interessado</t>
   </si>
@@ -71,6 +81,9 @@
   </si>
   <si>
     <t>Gerente de Configuração e Gerente de Projeto</t>
+  </si>
+  <si>
+    <t>Fim de Checklist</t>
   </si>
 </sst>
 </file>
@@ -121,16 +134,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -166,9 +179,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -206,7 +219,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -278,7 +291,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -454,18 +467,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="51.28515625" customWidth="1"/>
-    <col min="3" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="102.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="3" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="102.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -479,145 +492,157 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3">
+        <v>42128</v>
+      </c>
       <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>42128</v>
+      </c>
       <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>42129</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3">
+        <v>42135</v>
+      </c>
       <c r="E7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3">
+        <v>42129</v>
+      </c>
       <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="3"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>

</xml_diff>